<commit_message>
fix some manual selection; add practice list
</commit_message>
<xml_diff>
--- a/experiments/openai_production_adj_selection_manualdone.xlsx
+++ b/experiments/openai_production_adj_selection_manualdone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiangtianli/Projects/Yibin/state_overspec_modeling/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F8BA2065-88B0-5041-95AD-F91E4F8E3A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4148E6-5576-2D45-B488-C731CA203BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7DC31C8C-D523-294E-8456-16A64FB7E20B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{7DC31C8C-D523-294E-8456-16A64FB7E20B}"/>
   </bookViews>
   <sheets>
     <sheet name="openai_production_adj_selection" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="918">
   <si>
     <t>item</t>
   </si>
@@ -3421,9 +3421,6 @@
     <t>intact</t>
   </si>
   <si>
-    <t>U-shaped</t>
-  </si>
-  <si>
     <t>winding</t>
   </si>
   <si>
@@ -3451,9 +3448,6 @@
     <t>unlit</t>
   </si>
   <si>
-    <t>sharpened</t>
-  </si>
-  <si>
     <t>ripped</t>
   </si>
   <si>
@@ -3476,9 +3470,6 @@
   </si>
   <si>
     <t>capped</t>
-  </si>
-  <si>
-    <t>old</t>
   </si>
   <si>
     <t>lidded</t>
@@ -4348,8 +4339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A063289-9B2A-AA43-82BA-A8BD4491AC0B}">
   <dimension ref="A1:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="132" zoomScaleNormal="158" workbookViewId="0">
-      <selection activeCell="N55" sqref="N55"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="132" zoomScaleNormal="158" workbookViewId="0">
+      <selection activeCell="O96" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4411,7 +4402,7 @@
         <v>872</v>
       </c>
       <c r="P1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q1" t="s">
         <v>873</v>
@@ -4458,7 +4449,7 @@
         <v>874</v>
       </c>
       <c r="O2" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4548,9 +4539,6 @@
       <c r="O4" t="s">
         <v>877</v>
       </c>
-      <c r="P4" t="s">
-        <v>878</v>
-      </c>
     </row>
     <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -4681,7 +4669,7 @@
         <v>880</v>
       </c>
       <c r="O7" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4769,7 +4757,7 @@
         <v>875</v>
       </c>
       <c r="O9" t="s">
-        <v>919</v>
+        <v>876</v>
       </c>
       <c r="P9" t="s">
         <v>878</v>
@@ -5344,7 +5332,7 @@
         <v>880</v>
       </c>
       <c r="O22" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5435,7 +5423,7 @@
         <v>875</v>
       </c>
       <c r="O24" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -5611,7 +5599,7 @@
         <v>875</v>
       </c>
       <c r="O28" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -6317,6 +6305,9 @@
       <c r="N44" t="s">
         <v>887</v>
       </c>
+      <c r="O44" t="s">
+        <v>889</v>
+      </c>
       <c r="P44" t="s">
         <v>878</v>
       </c>
@@ -7031,7 +7022,10 @@
         <v>898</v>
       </c>
       <c r="O60" t="s">
-        <v>900</v>
+        <v>896</v>
+      </c>
+      <c r="P60" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7072,7 +7066,7 @@
         <v>526</v>
       </c>
       <c r="N61" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="O61" t="s">
         <v>896</v>
@@ -7116,7 +7110,7 @@
         <v>535</v>
       </c>
       <c r="N62" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="O62" t="s">
         <v>896</v>
@@ -7160,10 +7154,10 @@
         <v>546</v>
       </c>
       <c r="N63" t="s">
+        <v>902</v>
+      </c>
+      <c r="O63" t="s">
         <v>903</v>
-      </c>
-      <c r="O63" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="64" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7204,10 +7198,10 @@
         <v>546</v>
       </c>
       <c r="N64" t="s">
+        <v>902</v>
+      </c>
+      <c r="O64" t="s">
         <v>903</v>
-      </c>
-      <c r="O64" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7248,10 +7242,10 @@
         <v>546</v>
       </c>
       <c r="N65" t="s">
+        <v>902</v>
+      </c>
+      <c r="O65" t="s">
         <v>903</v>
-      </c>
-      <c r="O65" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7292,10 +7286,10 @@
         <v>546</v>
       </c>
       <c r="N66" t="s">
+        <v>902</v>
+      </c>
+      <c r="O66" t="s">
         <v>903</v>
-      </c>
-      <c r="O66" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7336,10 +7330,10 @@
         <v>546</v>
       </c>
       <c r="N67" t="s">
+        <v>902</v>
+      </c>
+      <c r="O67" t="s">
         <v>903</v>
-      </c>
-      <c r="O67" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="68" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7380,10 +7374,10 @@
         <v>546</v>
       </c>
       <c r="N68" t="s">
+        <v>902</v>
+      </c>
+      <c r="O68" t="s">
         <v>903</v>
-      </c>
-      <c r="O68" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="69" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7424,10 +7418,10 @@
         <v>594</v>
       </c>
       <c r="N69" t="s">
+        <v>902</v>
+      </c>
+      <c r="O69" t="s">
         <v>903</v>
-      </c>
-      <c r="O69" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7468,10 +7462,10 @@
         <v>546</v>
       </c>
       <c r="N70" t="s">
+        <v>902</v>
+      </c>
+      <c r="O70" t="s">
         <v>903</v>
-      </c>
-      <c r="O70" t="s">
-        <v>905</v>
       </c>
       <c r="P70" t="s">
         <v>878</v>
@@ -7515,10 +7509,10 @@
         <v>546</v>
       </c>
       <c r="N71" t="s">
+        <v>902</v>
+      </c>
+      <c r="O71" t="s">
         <v>903</v>
-      </c>
-      <c r="O71" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7559,10 +7553,10 @@
         <v>546</v>
       </c>
       <c r="N72" t="s">
+        <v>902</v>
+      </c>
+      <c r="O72" t="s">
         <v>903</v>
-      </c>
-      <c r="O72" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7603,10 +7597,10 @@
         <v>546</v>
       </c>
       <c r="N73" t="s">
+        <v>902</v>
+      </c>
+      <c r="O73" t="s">
         <v>903</v>
-      </c>
-      <c r="O73" t="s">
-        <v>905</v>
       </c>
       <c r="P73" t="s">
         <v>878</v>
@@ -7650,10 +7644,10 @@
         <v>546</v>
       </c>
       <c r="N74" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="O74" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7694,10 +7688,10 @@
         <v>642</v>
       </c>
       <c r="N75" t="s">
+        <v>902</v>
+      </c>
+      <c r="O75" t="s">
         <v>903</v>
-      </c>
-      <c r="O75" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="76" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7738,10 +7732,10 @@
         <v>546</v>
       </c>
       <c r="N76" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="O76" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="77" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -7782,7 +7776,7 @@
         <v>661</v>
       </c>
       <c r="N77" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O77" t="s">
         <v>883</v>
@@ -7826,7 +7820,7 @@
         <v>661</v>
       </c>
       <c r="N78" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O78" t="s">
         <v>883</v>
@@ -7870,7 +7864,7 @@
         <v>661</v>
       </c>
       <c r="N79" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O79" t="s">
         <v>883</v>
@@ -7914,7 +7908,7 @@
         <v>661</v>
       </c>
       <c r="N80" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O80" t="s">
         <v>899</v>
@@ -7958,10 +7952,10 @@
         <v>661</v>
       </c>
       <c r="N81" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O81" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="P81" t="s">
         <v>878</v>
@@ -8005,7 +7999,7 @@
         <v>661</v>
       </c>
       <c r="N82" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O82" t="s">
         <v>883</v>
@@ -8049,7 +8043,7 @@
         <v>661</v>
       </c>
       <c r="N83" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O83" t="s">
         <v>899</v>
@@ -8093,10 +8087,10 @@
         <v>661</v>
       </c>
       <c r="N84" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O84" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
       <c r="P84" t="s">
         <v>878</v>
@@ -8146,7 +8140,7 @@
         <v>892</v>
       </c>
       <c r="O85" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="86" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8187,10 +8181,10 @@
         <v>661</v>
       </c>
       <c r="N86" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O86" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8231,10 +8225,10 @@
         <v>661</v>
       </c>
       <c r="N87" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O87" t="s">
-        <v>910</v>
+        <v>899</v>
       </c>
       <c r="P87" t="s">
         <v>878</v>
@@ -8278,7 +8272,7 @@
         <v>661</v>
       </c>
       <c r="N88" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O88" t="s">
         <v>899</v>
@@ -8322,10 +8316,10 @@
         <v>661</v>
       </c>
       <c r="N89" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O89" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
       <c r="P89" t="s">
         <v>878</v>
@@ -8369,7 +8363,7 @@
         <v>661</v>
       </c>
       <c r="N90" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O90" t="s">
         <v>899</v>
@@ -8413,7 +8407,7 @@
         <v>661</v>
       </c>
       <c r="N91" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="O91" t="s">
         <v>899</v>
@@ -8501,7 +8495,7 @@
         <v>790</v>
       </c>
       <c r="N93" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="O93" t="s">
         <v>883</v>
@@ -8589,10 +8583,10 @@
         <v>790</v>
       </c>
       <c r="N95" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="O95" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="96" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8680,10 +8674,10 @@
         <v>826</v>
       </c>
       <c r="N97" t="s">
+        <v>911</v>
+      </c>
+      <c r="O97" t="s">
         <v>913</v>
-      </c>
-      <c r="O97" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="98" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8724,10 +8718,10 @@
         <v>835</v>
       </c>
       <c r="N98" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="O98" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="99" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8768,10 +8762,10 @@
         <v>844</v>
       </c>
       <c r="N99" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="O99" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="100" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8812,10 +8806,10 @@
         <v>825</v>
       </c>
       <c r="N100" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="O100" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="101" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8859,10 +8853,10 @@
         <v>861</v>
       </c>
       <c r="N101" t="s">
+        <v>911</v>
+      </c>
+      <c r="O101" t="s">
         <v>913</v>
-      </c>
-      <c r="O101" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="102" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -8903,10 +8897,10 @@
         <v>870</v>
       </c>
       <c r="N102" t="s">
+        <v>911</v>
+      </c>
+      <c r="O102" t="s">
         <v>913</v>
-      </c>
-      <c r="O102" t="s">
-        <v>915</v>
       </c>
     </row>
   </sheetData>

</xml_diff>